<commit_message>
Revert "edited excel files"
This reverts commit 56cb3c49ac803a6bcaffcaacfacb6e83f5cf3a80.
</commit_message>
<xml_diff>
--- a/Routers_data.xlsx
+++ b/Routers_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5BD6CA-1F8C-44E7-92C5-10E8C44AC30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E560E75-F1D8-4C07-8930-8D49E291E178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12255" yWindow="3150" windowWidth="14475" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,16 +49,16 @@
     <t>Interface</t>
   </si>
   <si>
-    <t>192.168.11.1/24</t>
-  </si>
-  <si>
-    <t>192.168.11.2/24</t>
-  </si>
-  <si>
-    <t>192.168.10.1/24</t>
-  </si>
-  <si>
-    <t>10.1.1.1/24</t>
+    <t>192.168.11.1</t>
+  </si>
+  <si>
+    <t>192.168.11.2</t>
+  </si>
+  <si>
+    <t>192.168.10.1</t>
+  </si>
+  <si>
+    <t>10.1.1.1</t>
   </si>
 </sst>
 </file>
@@ -457,18 +457,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="1" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -528,7 +528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -548,7 +548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -579,7 +579,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -591,7 +591,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>